<commit_message>
Add readme files and python debug
</commit_message>
<xml_diff>
--- a/APYTHON/uploads/liste_etudiant.xlsx
+++ b/APYTHON/uploads/liste_etudiant.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/spestana/Documents/EFREI/Advanced Programming/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A9DC4D-DA50-3946-BBA3-3108C1E7EF96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E2DB95-A2FC-814C-BB6E-0411A3EA1869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{AD8E3AB7-9284-CA47-8962-E718351E3667}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="60">
   <si>
     <t>nom</t>
   </si>
@@ -138,13 +138,91 @@
   </si>
   <si>
     <t>coursNom</t>
+  </si>
+  <si>
+    <t>juan@etudiant.com</t>
+  </si>
+  <si>
+    <t>maria@etudiant.com</t>
+  </si>
+  <si>
+    <t>carlos@etudiant.com</t>
+  </si>
+  <si>
+    <t>ana@etudiant.com</t>
+  </si>
+  <si>
+    <t>luis@etudiant.com</t>
+  </si>
+  <si>
+    <t>juan@ejemplo.com</t>
+  </si>
+  <si>
+    <t>maria@ejemplo.com</t>
+  </si>
+  <si>
+    <t>carlos@ejemplo.com</t>
+  </si>
+  <si>
+    <t>ana@ejemplo.com</t>
+  </si>
+  <si>
+    <t>luis@ejemplo.com</t>
+  </si>
+  <si>
+    <t>ejemplo1@gmail.com</t>
+  </si>
+  <si>
+    <t>ejemplo2@gmail.com</t>
+  </si>
+  <si>
+    <t>ejemplo3@gmail.com</t>
+  </si>
+  <si>
+    <t>ejemplo4@gmail.com</t>
+  </si>
+  <si>
+    <t>ejemplo5@gmail.com</t>
+  </si>
+  <si>
+    <t>ejemplo6@gmail.com</t>
+  </si>
+  <si>
+    <t>ejemplo7@gmail.com</t>
+  </si>
+  <si>
+    <t>ejemplo8@gmail.com</t>
+  </si>
+  <si>
+    <t>555-1234568</t>
+  </si>
+  <si>
+    <t>555-1234569</t>
+  </si>
+  <si>
+    <t>555-1234570</t>
+  </si>
+  <si>
+    <t>555-1234571</t>
+  </si>
+  <si>
+    <t>555-1234572</t>
+  </si>
+  <si>
+    <t>555-1234573</t>
+  </si>
+  <si>
+    <t>555-1234574</t>
+  </si>
+  <si>
+    <t>555-1234575</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -154,6 +232,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -176,14 +262,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -516,10 +605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EC7363E-048A-4A42-A4D1-D6D8343D6BEA}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -570,8 +659,8 @@
       <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
+      <c r="D2" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
@@ -596,8 +685,8 @@
       <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
-        <v>14</v>
+      <c r="D3" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="E3" t="s">
         <v>15</v>
@@ -622,8 +711,8 @@
       <c r="C4" t="s">
         <v>18</v>
       </c>
-      <c r="D4" t="s">
-        <v>19</v>
+      <c r="D4" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="E4" t="s">
         <v>20</v>
@@ -648,8 +737,8 @@
       <c r="C5" t="s">
         <v>23</v>
       </c>
-      <c r="D5" t="s">
-        <v>24</v>
+      <c r="D5" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>
@@ -674,8 +763,8 @@
       <c r="C6" t="s">
         <v>28</v>
       </c>
-      <c r="D6" t="s">
-        <v>29</v>
+      <c r="D6" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="E6" t="s">
         <v>30</v>
@@ -700,8 +789,8 @@
       <c r="C7" t="s">
         <v>7</v>
       </c>
-      <c r="D7" t="s">
-        <v>8</v>
+      <c r="D7" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="E7" t="s">
         <v>9</v>
@@ -726,8 +815,8 @@
       <c r="C8" t="s">
         <v>13</v>
       </c>
-      <c r="D8" t="s">
-        <v>14</v>
+      <c r="D8" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="E8" t="s">
         <v>15</v>
@@ -752,8 +841,8 @@
       <c r="C9" t="s">
         <v>18</v>
       </c>
-      <c r="D9" t="s">
-        <v>19</v>
+      <c r="D9" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="E9" t="s">
         <v>20</v>
@@ -778,8 +867,8 @@
       <c r="C10" t="s">
         <v>23</v>
       </c>
-      <c r="D10" t="s">
-        <v>24</v>
+      <c r="D10" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="E10" t="s">
         <v>25</v>
@@ -804,8 +893,8 @@
       <c r="C11" t="s">
         <v>28</v>
       </c>
-      <c r="D11" t="s">
-        <v>29</v>
+      <c r="D11" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="E11" t="s">
         <v>30</v>
@@ -1028,8 +1117,239 @@
         <v>11</v>
       </c>
     </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>20220252</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E20" t="s">
+        <v>52</v>
+      </c>
+      <c r="F20" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="1">
+        <v>36631</v>
+      </c>
+      <c r="H20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20220253</v>
+      </c>
+      <c r="B21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="1">
+        <v>36363</v>
+      </c>
+      <c r="H21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>20220254</v>
+      </c>
+      <c r="B22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" t="s">
+        <v>54</v>
+      </c>
+      <c r="F22" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" s="1">
+        <v>37144</v>
+      </c>
+      <c r="H22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>20220255</v>
+      </c>
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E23" t="s">
+        <v>55</v>
+      </c>
+      <c r="F23" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="1">
+        <v>37590</v>
+      </c>
+      <c r="H23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>20220256</v>
+      </c>
+      <c r="B24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E24" t="s">
+        <v>56</v>
+      </c>
+      <c r="F24" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="1">
+        <v>37685</v>
+      </c>
+      <c r="H24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>20220257</v>
+      </c>
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E25" t="s">
+        <v>57</v>
+      </c>
+      <c r="F25" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" s="1">
+        <v>36631</v>
+      </c>
+      <c r="H25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>20220258</v>
+      </c>
+      <c r="B26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E26" t="s">
+        <v>58</v>
+      </c>
+      <c r="F26" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" s="1">
+        <v>36363</v>
+      </c>
+      <c r="H26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>20220259</v>
+      </c>
+      <c r="B27" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" t="s">
+        <v>18</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E27" t="s">
+        <v>59</v>
+      </c>
+      <c r="F27" t="s">
+        <v>10</v>
+      </c>
+      <c r="G27" s="1">
+        <v>37144</v>
+      </c>
+      <c r="H27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G28" s="1"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{A70D32FF-7CA9-D04D-AAAF-28B39DB0E7A9}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{9F77B0F9-E6D0-AB4E-AED6-0B576695B78F}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{061A1813-8E19-034D-91BC-4FAC967CA069}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{6F9AC89D-0872-DD4E-A5E9-3FB2E6EE7146}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{47649399-5B36-B940-A0FE-1B892CD2FA18}"/>
+    <hyperlink ref="D7" r:id="rId6" xr:uid="{68F96FFD-4A9D-BA4A-BE0B-4811E28288A1}"/>
+    <hyperlink ref="D8" r:id="rId7" xr:uid="{AB1F651D-1D06-F548-AD1F-52874A985EC2}"/>
+    <hyperlink ref="D9" r:id="rId8" xr:uid="{8785466E-2C9C-A440-A0A7-6A7A32A8DDE2}"/>
+    <hyperlink ref="D10" r:id="rId9" xr:uid="{771AD8B5-01A3-554F-B26B-9B1D3EC538E7}"/>
+    <hyperlink ref="D11" r:id="rId10" xr:uid="{A725D696-B876-8944-9C74-88591C0204CB}"/>
+    <hyperlink ref="D20" r:id="rId11" xr:uid="{7562946B-9B8A-0647-9568-FF6AFAAE6B7B}"/>
+    <hyperlink ref="D21" r:id="rId12" xr:uid="{54CCFFC1-0A55-AB47-821D-DD54119FF7ED}"/>
+    <hyperlink ref="D22" r:id="rId13" xr:uid="{632A43D1-E860-2949-B775-0536552F9FE2}"/>
+    <hyperlink ref="D23" r:id="rId14" xr:uid="{C6AA5035-C86B-3A4E-900F-AB0729AFE21D}"/>
+    <hyperlink ref="D24" r:id="rId15" xr:uid="{F35C2AFD-FB10-D847-A3DB-958A61022CCE}"/>
+    <hyperlink ref="D25" r:id="rId16" xr:uid="{ECFF0AB8-8BE0-8447-AF1E-AE23A7FB6D6F}"/>
+    <hyperlink ref="D26" r:id="rId17" xr:uid="{4F64626D-4ECD-C44D-BBB2-5BAA7520A11C}"/>
+    <hyperlink ref="D27" r:id="rId18" xr:uid="{7C82F0C1-C23C-5A4B-AFA3-BE1438E96D55}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>